<commit_message>
chnages the pie to 2D
</commit_message>
<xml_diff>
--- a/sources/users_sheet.xlsx
+++ b/sources/users_sheet.xlsx
@@ -301,44 +301,8 @@
       </c:spPr>
     </c:title>
     <c:autoTitleDeleted val="0"/>
-    <c:view3D>
-      <c:rotX val="30"/>
-      <c:rotY val="0"/>
-      <c:rAngAx val="0"/>
-      <c:perspective val="10"/>
-    </c:view3D>
-    <c:floor>
-      <c:spPr>
-        <a:solidFill>
-          <a:srgbClr val="d9d9d9"/>
-        </a:solidFill>
-        <a:ln w="0">
-          <a:noFill/>
-        </a:ln>
-      </c:spPr>
-    </c:floor>
-    <c:sideWall>
-      <c:spPr>
-        <a:solidFill>
-          <a:srgbClr val="d9d9d9"/>
-        </a:solidFill>
-        <a:ln w="0">
-          <a:noFill/>
-        </a:ln>
-      </c:spPr>
-    </c:sideWall>
-    <c:backWall>
-      <c:spPr>
-        <a:solidFill>
-          <a:srgbClr val="d9d9d9"/>
-        </a:solidFill>
-        <a:ln w="0">
-          <a:noFill/>
-        </a:ln>
-      </c:spPr>
-    </c:backWall>
     <c:plotArea>
-      <c:pie3DChart>
+      <c:pieChart>
         <c:varyColors val="1"/>
         <c:ser>
           <c:idx val="0"/>
@@ -410,7 +374,6 @@
                   </a:pPr>
                 </a:p>
               </c:txPr>
-              <c:dLblPos val="bestFit"/>
               <c:showLegendKey val="0"/>
               <c:showVal val="0"/>
               <c:showCatName val="0"/>
@@ -431,7 +394,6 @@
                   </a:pPr>
                 </a:p>
               </c:txPr>
-              <c:dLblPos val="bestFit"/>
               <c:showLegendKey val="0"/>
               <c:showVal val="0"/>
               <c:showCatName val="0"/>
@@ -452,7 +414,6 @@
                   </a:pPr>
                 </a:p>
               </c:txPr>
-              <c:dLblPos val="bestFit"/>
               <c:showLegendKey val="0"/>
               <c:showVal val="0"/>
               <c:showCatName val="0"/>
@@ -473,7 +434,6 @@
                   </a:pPr>
                 </a:p>
               </c:txPr>
-              <c:dLblPos val="bestFit"/>
               <c:showLegendKey val="0"/>
               <c:showVal val="0"/>
               <c:showCatName val="0"/>
@@ -492,7 +452,6 @@
                 </a:pPr>
               </a:p>
             </c:txPr>
-            <c:dLblPos val="bestFit"/>
             <c:showLegendKey val="0"/>
             <c:showVal val="0"/>
             <c:showCatName val="0"/>
@@ -531,7 +490,16 @@
             </c:numRef>
           </c:val>
         </c:ser>
-      </c:pie3DChart>
+        <c:firstSliceAng val="0"/>
+      </c:pieChart>
+      <c:spPr>
+        <a:solidFill>
+          <a:srgbClr val="d9d9d9"/>
+        </a:solidFill>
+        <a:ln w="0">
+          <a:noFill/>
+        </a:ln>
+      </c:spPr>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
@@ -555,7 +523,6 @@
       </c:txPr>
     </c:legend>
     <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="zero"/>
   </c:chart>
   <c:spPr>
     <a:solidFill>
@@ -579,9 +546,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>366120</xdr:colOff>
+      <xdr:colOff>365760</xdr:colOff>
       <xdr:row>21</xdr:row>
-      <xdr:rowOff>37440</xdr:rowOff>
+      <xdr:rowOff>37080</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -590,7 +557,7 @@
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="8461440" y="1490040"/>
-        <a:ext cx="5767920" cy="3239280"/>
+        <a:ext cx="5776560" cy="3238920"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -611,10 +578,10 @@
   <dimension ref="A1:I5"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="K4" activeCellId="0" sqref="K4"/>
+      <selection pane="topLeft" activeCell="D11" activeCellId="0" sqref="D11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="17.35" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="17.35" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="1" style="1" width="28.9"/>
   </cols>

</xml_diff>